<commit_message>
add: se prepara para hacer merge a develop
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\proyectogrupal1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65D5D59-5A2E-4C1C-8E48-8B8EDCABE9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A1717A-EDCA-4553-8DE8-0CE9924BA8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>cond</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Constante</t>
+  </si>
+  <si>
+    <t>Modulo</t>
+  </si>
+  <si>
+    <t>Exponencial</t>
   </si>
 </sst>
 </file>
@@ -169,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -183,11 +189,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -224,7 +233,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>408925</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>172169</xdr:rowOff>
+      <xdr:rowOff>66152</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -557,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98BBD8C-B9E8-4C66-8139-ABC2780EC3EF}">
-  <dimension ref="B2:E7"/>
+  <dimension ref="A2:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,16 +577,16 @@
     <col min="5" max="5" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="6" t="s">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -591,7 +600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -605,7 +614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
       <c r="C6" s="4">
         <v>10</v>
@@ -617,16 +626,84 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
+    <row r="7" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="5"/>
-    </row>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add: se compila a la fpga, se encuentra bug con branch en la fpga, en simulacion sirve
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\proyectogrupal1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A1717A-EDCA-4553-8DE8-0CE9924BA8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14244F8F-6643-49F1-9FC7-3D4DB4497315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>cond</t>
   </si>
@@ -59,9 +59,6 @@
     <t>23:0</t>
   </si>
   <si>
-    <t>label = InstrDest - InstrSrc</t>
-  </si>
-  <si>
     <t>Branchs</t>
   </si>
   <si>
@@ -75,13 +72,19 @@
   </si>
   <si>
     <t>Exponencial</t>
+  </si>
+  <si>
+    <t>PC Destino</t>
+  </si>
+  <si>
+    <t>Simplemente es la linea de la instr destino</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +111,13 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -175,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,15 +199,16 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,7 +580,7 @@
   <dimension ref="A2:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,12 +590,12 @@
   <sheetData>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
@@ -597,7 +608,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -623,23 +634,26 @@
         <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="6"/>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
@@ -652,7 +666,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -662,20 +676,20 @@
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
@@ -688,7 +702,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
add: se eliminan elementos que no se usan
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\proyectogrupal1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14244F8F-6643-49F1-9FC7-3D4DB4497315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9D907F-C291-443B-8E01-85220EA6B154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
   <si>
     <t>cond</t>
   </si>
@@ -68,23 +69,161 @@
     <t>Constante</t>
   </si>
   <si>
-    <t>Modulo</t>
-  </si>
-  <si>
-    <t>Exponencial</t>
-  </si>
-  <si>
     <t>PC Destino</t>
   </si>
   <si>
     <t>Simplemente es la linea de la instr destino</t>
+  </si>
+  <si>
+    <t>OPCODE</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>31:30</t>
+  </si>
+  <si>
+    <t>JMP</t>
+  </si>
+  <si>
+    <t>JEQ</t>
+  </si>
+  <si>
+    <t>JNE</t>
+  </si>
+  <si>
+    <t>29:28</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Label de salto</t>
+  </si>
+  <si>
+    <t>27:0</t>
+  </si>
+  <si>
+    <t>Datos</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>SUB</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>CMP</t>
+  </si>
+  <si>
+    <t>ADDI</t>
+  </si>
+  <si>
+    <t>SUBI</t>
+  </si>
+  <si>
+    <t>ANDI</t>
+  </si>
+  <si>
+    <t>ORI</t>
+  </si>
+  <si>
+    <t>CMPI</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>29:27</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>24:21</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>20:17</t>
+  </si>
+  <si>
+    <t>16:13</t>
+  </si>
+  <si>
+    <t>Immediate</t>
+  </si>
+  <si>
+    <t>12:0</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>24:0</t>
+  </si>
+  <si>
+    <t>Memoria</t>
+  </si>
+  <si>
+    <t>LDR</t>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,8 +261,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,8 +301,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF763C9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCB6F7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -181,11 +382,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,16 +450,123 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -217,6 +575,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFCB6F7"/>
+      <color rgb="FFF763C9"/>
       <color rgb="FFFFCCCC"/>
     </mruColors>
   </colors>
@@ -229,55 +589,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>12070</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>17511</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>408925</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>66152</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B2A7A67-F801-4FE8-FF0D-C0E88834DEC4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4690087" y="395198"/>
-          <a:ext cx="7102455" cy="7078919"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,150 +888,549 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98BBD8C-B9E8-4C66-8139-ABC2780EC3EF}">
-  <dimension ref="A2:F16"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="26.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="3" t="s">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="2">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E13" s="18"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="33"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="33"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="33"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="33"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="33"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="27"/>
+      <c r="B18" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="34"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="27"/>
+      <c r="B19" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="35"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="2"/>
-      <c r="C6" s="4">
+      <c r="E20" s="18"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="18"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="42"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="44"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E30" s="17"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="E31" s="17"/>
+    </row>
+    <row r="32" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B13:E13"/>
+  <mergeCells count="19">
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD358B2-7335-4163-8A2A-EBE61E673EB6}">
+  <dimension ref="A2:D7"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+      <c r="B6" s="4">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="B7:C7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add: se termina el refactor
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\proyectogrupal1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9D907F-C291-443B-8E01-85220EA6B154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C02812-E5BA-4A85-BE1D-58FB2A029482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
   </bookViews>
@@ -454,119 +454,117 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,6 +587,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>477078</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>340699</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>57507</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7C198B1-3071-DB3D-5A20-36F429B87588}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6420678" y="4903304"/>
+          <a:ext cx="9007621" cy="2217612"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>443948</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>26504</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>414205</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>32064</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A567A02-A2ED-9D1C-A1CC-FC955DF14A03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6379928" y="1786724"/>
+          <a:ext cx="8504657" cy="2977360"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -890,26 +981,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98BBD8C-B9E8-4C66-8139-ABC2780EC3EF}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
     </row>
     <row r="3" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
@@ -918,418 +1009,430 @@
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="14"/>
+      <c r="E4" s="41"/>
     </row>
     <row r="5" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="17"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="36"/>
     </row>
     <row r="7" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="36"/>
     </row>
     <row r="8" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="23" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="32" t="s">
+      <c r="H12" s="23" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="16" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
       </c>
-      <c r="E13" s="18"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="33"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
       </c>
-      <c r="E14" s="18"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="33"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="11" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
       </c>
-      <c r="E15" s="18"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="33"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="24"/>
     </row>
     <row r="16" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="16" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
       </c>
-      <c r="E16" s="18"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="33"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="11" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
       </c>
-      <c r="E17" s="18"/>
+      <c r="E17" s="45"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="33"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="27"/>
-      <c r="B18" s="22" t="s">
+      <c r="A18" s="18"/>
+      <c r="B18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="34" t="s">
+      <c r="G18" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="H18" s="34"/>
+      <c r="H18" s="29"/>
     </row>
     <row r="19" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="27"/>
-      <c r="B19" s="29" t="s">
+      <c r="A19" s="18"/>
+      <c r="B19" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="35" t="s">
+      <c r="G19" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="35"/>
+      <c r="H19" s="30"/>
     </row>
     <row r="20" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
       </c>
-      <c r="E20" s="18"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
     </row>
     <row r="21" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
       </c>
-      <c r="E21" s="18"/>
+      <c r="E21" s="10"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
     </row>
     <row r="22" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
       </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
     </row>
     <row r="23" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
       </c>
-      <c r="E23" s="18"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="15" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
       </c>
-      <c r="E24" s="18"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
     </row>
     <row r="25" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
     </row>
     <row r="28" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="41" t="s">
+      <c r="C28" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="42"/>
+      <c r="E28" s="33"/>
     </row>
     <row r="29" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="44"/>
+      <c r="E29" s="34"/>
     </row>
     <row r="30" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="17"/>
+      <c r="E30" s="36"/>
     </row>
     <row r="31" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="17"/>
+      <c r="E31" s="36"/>
     </row>
     <row r="32" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="G18:H18"/>
@@ -1337,21 +1440,10 @@
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G22:H22"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1370,12 +1462,12 @@
   <sheetData>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
     </row>
     <row r="4" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -1418,10 +1510,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="6" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
add: primera version del pipeline con isa nuevo, errores con inst mem
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\proyectogrupal1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F711C78-6D05-49F6-9C3B-9199E2389523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F65C6B-91AE-44F5-AFE7-2DCC756BCD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
   </bookViews>
@@ -762,6 +762,48 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -771,99 +813,6 @@
     <xf numFmtId="0" fontId="2" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -872,21 +821,72 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1219,7 +1219,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,16 +1238,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.399999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="83"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="43"/>
     </row>
     <row r="2" spans="1:9" ht="10.8" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:9" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1285,27 +1285,27 @@
     </row>
     <row r="6" spans="1:9" ht="10.199999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:9" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="79"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62"/>
     </row>
     <row r="8" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="63" t="s">
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="64"/>
-      <c r="G8" s="65"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="77"/>
       <c r="H8" s="13" t="s">
         <v>54</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>33</v>
@@ -1387,7 +1387,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>34</v>
@@ -1413,7 +1413,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>35</v>
@@ -1439,7 +1439,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>36</v>
@@ -1465,7 +1465,7 @@
         <v>83</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>37</v>
@@ -1491,7 +1491,7 @@
         <v>85</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>84</v>
@@ -1517,7 +1517,7 @@
         <v>86</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>87</v>
@@ -1543,7 +1543,7 @@
         <v>26</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>88</v>
@@ -1576,29 +1576,29 @@
     </row>
     <row r="20" spans="1:8" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="23"/>
-      <c r="B20" s="70" t="s">
+      <c r="B20" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="72"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="82"/>
     </row>
     <row r="21" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="23"/>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="67" t="s">
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="69"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="50"/>
     </row>
     <row r="22" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="23"/>
@@ -1617,10 +1617,10 @@
       <c r="F22" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="67" t="s">
+      <c r="G22" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="69"/>
+      <c r="H22" s="50"/>
     </row>
     <row r="23" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="23"/>
@@ -1639,17 +1639,17 @@
       <c r="F23" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="G23" s="75" t="s">
+      <c r="G23" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="H23" s="76"/>
+      <c r="H23" s="52"/>
     </row>
     <row r="24" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="33" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>33</v>
@@ -1663,17 +1663,17 @@
       <c r="F24" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="50" t="s">
+      <c r="G24" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="H24" s="51"/>
+      <c r="H24" s="45"/>
     </row>
     <row r="25" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="33" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>34</v>
@@ -1687,17 +1687,17 @@
       <c r="F25" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="50" t="s">
+      <c r="G25" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="H25" s="51"/>
+      <c r="H25" s="45"/>
     </row>
     <row r="26" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="33" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>35</v>
@@ -1711,17 +1711,17 @@
       <c r="F26" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="50" t="s">
+      <c r="G26" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="H26" s="51"/>
+      <c r="H26" s="45"/>
     </row>
     <row r="27" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="33" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>36</v>
@@ -1735,20 +1735,20 @@
       <c r="F27" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G27" s="50" t="s">
+      <c r="G27" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="H27" s="51"/>
+      <c r="H27" s="45"/>
     </row>
     <row r="28" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="33" t="s">
         <v>83</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D28" s="22">
         <v>1</v>
@@ -1759,20 +1759,20 @@
       <c r="F28" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="50" t="s">
+      <c r="G28" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="H28" s="51"/>
+      <c r="H28" s="45"/>
     </row>
     <row r="29" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="33" t="s">
         <v>85</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="D29" s="22">
         <v>1</v>
@@ -1783,20 +1783,20 @@
       <c r="F29" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G29" s="50" t="s">
+      <c r="G29" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="H29" s="51"/>
+      <c r="H29" s="45"/>
     </row>
     <row r="30" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="33" t="s">
         <v>86</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="D30" s="22">
         <v>1</v>
@@ -1807,20 +1807,20 @@
       <c r="F30" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G30" s="50" t="s">
+      <c r="G30" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="H30" s="51"/>
+      <c r="H30" s="45"/>
     </row>
     <row r="31" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="33" t="s">
         <v>31</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="D31" s="22">
         <v>1</v>
@@ -1831,35 +1831,35 @@
       <c r="F31" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G31" s="50" t="s">
+      <c r="G31" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="H31" s="51"/>
+      <c r="H31" s="45"/>
     </row>
     <row r="32" spans="1:8" ht="11.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="33" spans="1:8" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="53" t="s">
+      <c r="B33" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
     </row>
     <row r="34" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="73" t="s">
+      <c r="B34" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
-      <c r="E34" s="52" t="s">
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
     </row>
     <row r="35" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="34" t="s">
@@ -1877,10 +1877,10 @@
       <c r="F35" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="G35" s="44" t="s">
+      <c r="G35" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="H35" s="45"/>
+      <c r="H35" s="59"/>
     </row>
     <row r="36" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="36" t="s">
@@ -1898,10 +1898,10 @@
       <c r="F36" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="G36" s="74" t="s">
+      <c r="G36" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="H36" s="74"/>
+      <c r="H36" s="55"/>
     </row>
     <row r="37" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="38" t="s">
@@ -1922,10 +1922,10 @@
       <c r="F37" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="G37" s="43" t="s">
+      <c r="G37" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="H37" s="43"/>
+      <c r="H37" s="57"/>
     </row>
     <row r="38" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="39" t="s">
@@ -1946,37 +1946,37 @@
       <c r="F38" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="G38" s="43" t="s">
+      <c r="G38" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="H38" s="43"/>
+      <c r="H38" s="57"/>
     </row>
     <row r="39" spans="1:8" ht="11.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="40" spans="1:8" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="49" t="s">
+      <c r="B40" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="49"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="49"/>
-      <c r="H40" s="49"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="69"/>
     </row>
     <row r="41" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="80" t="s">
+      <c r="B41" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="80"/>
-      <c r="D41" s="80"/>
-      <c r="E41" s="54" t="s">
+      <c r="C41" s="56"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="F41" s="54"/>
-      <c r="G41" s="56" t="s">
+      <c r="F41" s="68"/>
+      <c r="G41" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="H41" s="57"/>
+      <c r="H41" s="65"/>
     </row>
     <row r="42" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="7" t="s">
@@ -1988,14 +1988,14 @@
       <c r="D42" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="54" t="s">
+      <c r="E42" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="F42" s="54"/>
-      <c r="G42" s="56" t="s">
+      <c r="F42" s="68"/>
+      <c r="G42" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="H42" s="57"/>
+      <c r="H42" s="65"/>
     </row>
     <row r="43" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="8" t="s">
@@ -2007,21 +2007,21 @@
       <c r="D43" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="54" t="s">
+      <c r="E43" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="F43" s="54"/>
-      <c r="G43" s="58" t="s">
+      <c r="F43" s="68"/>
+      <c r="G43" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="H43" s="59"/>
+      <c r="H43" s="67"/>
     </row>
     <row r="44" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>19</v>
@@ -2029,19 +2029,19 @@
       <c r="D44" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="55" t="s">
+      <c r="E44" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="F44" s="55"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="51"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="45"/>
     </row>
     <row r="45" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>20</v>
@@ -2049,19 +2049,19 @@
       <c r="D45" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="E45" s="55" t="s">
+      <c r="E45" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="F45" s="55"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="51"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="45"/>
     </row>
     <row r="46" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>21</v>
@@ -2069,22 +2069,18 @@
       <c r="D46" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="E46" s="55" t="s">
+      <c r="E46" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="F46" s="55"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="51"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="45"/>
     </row>
     <row r="47" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="B21:D21"/>
     <mergeCell ref="E21:H21"/>
     <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B7:H7"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="G42:H42"/>
@@ -2100,6 +2096,7 @@
     <mergeCell ref="B33:H33"/>
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="E44:F44"/>
+    <mergeCell ref="B8:D8"/>
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="G36:H36"/>
@@ -2107,6 +2104,9 @@
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
@@ -2117,9 +2117,9 @@
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="B21:D21"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2142,12 +2142,12 @@
   <sheetData>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
     </row>
     <row r="4" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -2190,10 +2190,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="82"/>
+      <c r="C7" s="84"/>
       <c r="D7" s="5" t="s">
         <v>11</v>
       </c>

</xml_diff>